<commit_message>
Updated code of OOH PBT BOT
</commit_message>
<xml_diff>
--- a/OOH_PBT/OOH_PBT_Dispatcher/Data/Config.xlsx
+++ b/OOH_PBT/OOH_PBT_Dispatcher/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1files\UPProjects\OOH_PBT\OOH_PBT_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Files\UPProjects\OOH_PBT\OOH_PBT_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC523867-1087-485D-9508-69D77734C87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E192C8-4180-46DA-956D-668FA0F7D863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="14670" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -120,60 +120,12 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>ToolkitPasswordBackup</t>
-  </si>
-  <si>
-    <t>2GKV7TS7Qd</t>
-  </si>
-  <si>
-    <t>RunSheet_Template_Path</t>
-  </si>
-  <si>
-    <t>RunSheet_Path</t>
-  </si>
-  <si>
-    <t>PBT Queue</t>
-  </si>
-  <si>
-    <t>Queue used in the Dispatcher Bot</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>PBTLoginCredential</t>
   </si>
   <si>
-    <t>PBTLogFileDate</t>
-  </si>
-  <si>
-    <t>Used to configure the date of the Log File to be picked</t>
-  </si>
-  <si>
-    <t>/Bot%20Ready/</t>
-  </si>
-  <si>
-    <t>in_sharepoint_Download_Folder_main</t>
-  </si>
-  <si>
-    <t>in_Log_file_folder_path_main</t>
-  </si>
-  <si>
-    <t>/Processed/</t>
-  </si>
-  <si>
-    <t>TemplateLogFile</t>
-  </si>
-  <si>
     <t>MultiBuyPDFPath</t>
   </si>
   <si>
-    <t>FANames</t>
-  </si>
-  <si>
-    <t>Erin.Mckenna,Anthony.Plakas</t>
-  </si>
-  <si>
     <t>SQLDatabaseConnectionString</t>
   </si>
   <si>
@@ -183,21 +135,6 @@
     <t>System.Data.SqlClient</t>
   </si>
   <si>
-    <t>OrchestratorQueueNameFord</t>
-  </si>
-  <si>
-    <t>C:\Users\NTMGRM.RPA1\Desktop\Runsheet_Template.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\NTMGRM.RPA1\Desktop\Runsheet.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\NTMGRM.RPA1\Desktop\LogFiles\</t>
-  </si>
-  <si>
-    <t>C:\Users\NTMGRM.RPA1\Downloads\PBT_Dispather_Performer_Model\Main_Dispatcher\Data\InvoiceLog_Template.xlsx</t>
-  </si>
-  <si>
     <t>SharepointURL</t>
   </si>
   <si>
@@ -213,15 +150,9 @@
     <t>Data Source=eussqsvgrmusafinance01.database.windows.net;Initial Catalog=eussqdbgrmusaapoohdev01;User ID=NA_sqlusr_AP_OOH_DEV_01;Password=JFcRxniU2hETyEgCQxM3</t>
   </si>
   <si>
-    <t>APDigitalOOHPBTFord</t>
-  </si>
-  <si>
     <t>Login Credentials for OOH PBT Application</t>
   </si>
   <si>
-    <t>OOH PBT Queue</t>
-  </si>
-  <si>
     <t>https://insidemedia.sharepoint.com/sites/GMUSA-KineticFinanceAutomation/</t>
   </si>
   <si>
@@ -231,14 +162,14 @@
     <t>PBTLoginOOH</t>
   </si>
   <si>
-    <t>C:\1files\UPProjects\OOH_PBT\Download_Invoice\</t>
+    <t>C:\Users\NTMGRM.RPA1\Desktop\MultiBuy_Invoice\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -261,16 +192,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF4E5E65"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF4E5E65"/>
-      <name val="Roboto"/>
     </font>
     <font>
       <u/>
@@ -303,9 +224,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -315,13 +236,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -637,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -689,8 +608,8 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>66</v>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -698,13 +617,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
@@ -720,1242 +639,58 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>45</v>
+      <c r="A9" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2932,26 +1667,32 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2959,14 +1700,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2990,44 +1729,1131 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
+    <row r="2" spans="1:26" ht="30">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>40</v>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z995"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C9" s="5"/>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C11" s="6"/>
-    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4012,8 +3838,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded PBT Ford code
</commit_message>
<xml_diff>
--- a/OOH_PBT/OOH_PBT_Dispatcher/Data/Config.xlsx
+++ b/OOH_PBT/OOH_PBT_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Files\UPProjects\OOH_PBT\OOH_PBT_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E192C8-4180-46DA-956D-668FA0F7D863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98C685B-C68B-49C6-9E47-32A9119A2CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -126,9 +126,6 @@
     <t>MultiBuyPDFPath</t>
   </si>
   <si>
-    <t>SQLDatabaseConnectionString</t>
-  </si>
-  <si>
     <t>SQLDatabaseProviderName</t>
   </si>
   <si>
@@ -163,6 +160,24 @@
   </si>
   <si>
     <t>C:\Users\NTMGRM.RPA1\Desktop\MultiBuy_Invoice\</t>
+  </si>
+  <si>
+    <t>Data Source=eussqsvgrmusafinance01.database.windows.net;Initial Catalog=eussqdbgrmusaapooh01;User ID=NA_AP_OOH_DBAUSR_01;Password=n28UxD8NVZAqdFMjBHnd</t>
+  </si>
+  <si>
+    <t>SQLDatabaseConnectionStringProd</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueNameFord</t>
+  </si>
+  <si>
+    <t>AP_OOH_PBTFord</t>
+  </si>
+  <si>
+    <t>FordString</t>
+  </si>
+  <si>
+    <t>BLH,CRH,CRR,CHP,CCS,CCV,CPW,DLP,DDP,DIB,DSO,X20,DPI,DPN,YER,YFL,Z1C,FCP,FD,YA,YB,YBF,YC,YCA,YCD,YCL,YCM,YDF,YE,YEP,YER,YFV,YG,YH,YHU,YI,YJ,YK,YKC,YL,YLD,YM,YMD,YMO,YMR,YNA,YNE,YNM,YNW,YR,YSL,YTC,YTM,YTO,YTR,YTX,YWA,Y1A,Y1B,Y1C,Y1D,Y1E,Y1F,Y1G,Y1H,Y1I,Y1J,Y1K,Y1L,Y1M,Y1N,Y1O,Y1P,Y1Q,Y1R,Y1S,Y1T,Y1U,Y1V,Y1W,Y1X,Y1Y,Y1Z,ZA,ZAZ,ZB,ZC,ZCD,ZCM,ZFD,ZGR,ZH,ZID,ZIM,ZJ,ZLD,ZLM,ZLV,ZNE,ZR,ZSD,ZSF,ZT,ZTR,Z1A,Z1B,Z1D,Z1F,Z1G,Z1H,Z1I,Z1P,Z1S,Z1U,YA,YB,YBF,YCA,YCD,YCM,YDF,YEP,YFV,YG,YH,YHU,YI,YJ,YK,YL,YLD,YM,YNA,YNM,YNW,YR,YSL,YTM,YTO,YTX,YWA,L1H,THF,Z3A,Y3G,Y3N,Y3Q,Y3W,Z3G,Z3B,Z3D,Y3B,Y3E,Y3J,Y3X,Z3P,Y3D,Z3F,Z3H,Z3I,Z3U,L3H,Y3C,Y3A,Y3L,Y3M,Y3O,Y3F,Y3H,Y3I,Y3R,Y3T,Y3U,Y3V,Y3K,Y3P,Y3Y,Z3S,Y3Z,Z3C,FAR,MCO,MCS,MFA,MFC,MFD,MFE,MFG,MFL,MFM,MFO,MFR,MLA,MLR,MRM,MSM,MSP,MTO,FCP,FMR,MJ,JAR,JCX,MRO,LNC,MLD,MLM,MMD,MM,NSI,OAK,OHI,RBC,SMB,TAU,MTH,SMO,TSP,UNW,UNM,MUN,MVI,MVO</t>
   </si>
 </sst>
 </file>
@@ -226,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -241,6 +256,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -556,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -609,7 +627,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -620,10 +638,10 @@
         <v>31</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
@@ -642,7 +660,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -650,47 +668,56 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>42</v>
+      <c r="B8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
+      <c r="A9" t="s">
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="2"/>
+      <c r="A12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1668,11 +1695,10 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2794,7 +2820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
after Orchestrator migration code
</commit_message>
<xml_diff>
--- a/OOH_PBT/OOH_PBT_Dispatcher/Data/Config.xlsx
+++ b/OOH_PBT/OOH_PBT_Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Files\UPProjects\OOH_PBT\OOH_PBT_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.OOHPBTDIGS9\Documents\UiPath\OOH PBT\OOH_PBT_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92606A4-3011-4765-8DAB-FEE0F216C7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF94F98C-6A41-4169-9B67-215F5720EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -177,7 +177,13 @@
     <t>FordString</t>
   </si>
   <si>
-    <t>BLH,CRH,CRR,CHP,CCS,CCV,CPW,DLP,DDP,DIB,DSO,X20,DPI,DPN,YER,YFL,Z1C,FCP,FD,YA,YB,YBF,YC,YCA,YCD,YCL,YCM,YDF,YE,YEP,YER,YFV,YG,YH,YHU,YI,YJ,YK,YKC,YL,YLD,YM,YMD,YMO,YMR,YNA,YNE,YNM,YNW,YR,YSL,YTC,YTM,YTO,YTR,YTX,YWA,Y1A,Y1B,Y1C,Y1D,Y1E,Y1F,Y1G,Y1H,Y1I,Y1J,Y1K,Y1L,Y1M,Y1N,Y1O,Y1P,Y1Q,Y1R,Y1S,Y1T,Y1U,Y1V,Y1W,Y1X,Y1Y,Y1Z,ZA,ZAZ,ZB,ZC,ZCD,ZCM,ZFD,ZGR,ZH,ZID,ZIM,ZJ,ZLD,ZLM,ZLV,ZNE,ZR,ZSD,ZSF,ZT,ZTR,Z1A,Z1B,Z1D,Z1F,Z1G,Z1H,Z1I,Z1P,Z1S,Z1U,YA,YB,YBF,YCA,YCD,YCM,YDF,YEP,YFV,YG,YH,YHU,YI,YJ,YK,YL,YLD,YM,YNA,YNM,YNW,YR,YSL,YTM,YTO,YTX,YWA,L1H,THF,Z3A,Y3G,Y3N,Y3Q,Y3W,Z3G,Z3B,Z3D,Y3B,Y3E,Y3J,Y3X,Z3P,Y3D,Z3F,Z3H,Z3I,Z3U,L3H,Y3C,Y3A,Y3L,Y3M,Y3O,Y3F,Y3H,Y3I,Y3R,Y3T,Y3U,Y3V,Y3K,Y3P,Y3Y,Z3S,Y3Z,Z3C,FAR,MCO,MCS,MFA,MFC,MFD,MFE,MFG,MFL,MFM,MFO,MFR,MLA,MLR,MRM,MSM,MSP,MTO,FCP,FMR,MJ,JAR,JCX,MRO,LNC,MLD,MLM,MMD,MM,NSI,OAK,OHI,RBC,SMB,TAU,MTH,SMO,TSP,UNW,UNM,MUN,MVI,MVO,VFD</t>
+    <t>BLH,CRH,CRR,CHP,CCS,CCV,CPW,DLP,DDP,DIB,DSO,X20,DPI,DPN,YER,YFL,Z1C,FCP,FD,YA,YB,YBF,YC,YCA,YCD,YCL,YCM,YDF,YE,YEP,YER,YFV,YG,YH,YHU,YI,YJ,YK,YKC,YL,YLD,YM,YMD,YMO,YMR,YNA,YNE,YNM,YNW,YR,YSL,YTC,YTM,YTO,YTR,YTX,YWA,Y1A,Y1B,Y1C,Y1D,Y1E,Y1F,Y1G,Y1H,Y1I,Y1J,Y1K,Y1L,Y1M,Y1N,Y1O,Y1P,Y1Q,Y1R,Y1S,Y1T,Y1U,Y1V,Y1W,Y1X,Y1Y,Y1Z,ZA,ZAZ,ZB,ZC,ZCD,ZCM,ZFD,ZGR,ZH,ZID,ZIM,ZJ,ZLD,ZLM,ZLV,ZNE,ZR,ZSD,ZSF,ZT,ZTR,Z1A,Z1B,Z1D,Z1F,Z1G,Z1H,Z1I,Z1P,Z1S,Z1U,YA,YB,YBF,YCA,YCD,YCM,YDF,YEP,YFV,YG,YH,YHU,YI,YJ,YK,YL,YLD,YM,YNA,YNM,YNW,YR,YSL,YTM,YTO,YTX,YWA,L1H,THF,Z3A,Y3G,Y3N,Y3Q,Y3W,Z3G,Z3B,Z3D,Y3B,Y3E,Y3J,Y3X,Z3P,Y3D,Z3F,Z3H,Z3I,Z3U,L3H,Y3C,Y3A,Y3L,Y3M,Y3O,Y3F,Y3H,Y3I,Y3R,Y3T,Y3U,Y3V,Y3K,Y3P,Y3Y,Z3S,Y3Z,Z3C,FAR,MCO,MCS,MFA,MFC,MFD,MFE,MFG,MFL,MFM,MFO,MFR,MLA,MLR,MRM,MSM,MSP,MTO,FCP,FMR,MJ,JAR,JCX,MRO,LNC,MLD,MLM,MMD,MM,NSI,OAK,OHI,RBC,SMB,TAU,MTH,SMO,TSP,UNW,UNM,MUN,MVI,MVO,VFD,VLM</t>
+  </si>
+  <si>
+    <t>Cloud_FolderPath</t>
+  </si>
+  <si>
+    <t>GMUSA_PBTBOT</t>
   </si>
 </sst>
 </file>
@@ -241,24 +247,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -577,7 +580,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -704,22 +707,29 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3869,4 +3879,286 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010045A9A53AB2AD7C409EFC96CC55961B83" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="737d8429b8eb9892549b3c27dc155f66">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="649a79cd-06e4-47a3-aac9-21cb806f3675" xmlns:ns3="7f25b792-b2ba-4b5c-8669-b39a27555406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c35880a7ae30656a46222e88cc05a07" ns2:_="" ns3:_="">
+    <xsd:import namespace="649a79cd-06e4-47a3-aac9-21cb806f3675"/>
+    <xsd:import namespace="7f25b792-b2ba-4b5c-8669-b39a27555406"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:Time" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="649a79cd-06e4-47a3-aac9-21cb806f3675" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="cb8c6112-a551-416c-b446-07c3fc3d0d42" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="19" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Time" ma:index="20" nillable="true" ma:displayName="Time" ma:format="DateTime" ma:internalName="Time">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7f25b792-b2ba-4b5c-8669-b39a27555406" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="18" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{2e954b58-32a8-4cab-baf9-92d5046718f0}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7f25b792-b2ba-4b5c-8669-b39a27555406">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7f25b792-b2ba-4b5c-8669-b39a27555406" xsi:nil="true"/>
+    <Time xmlns="649a79cd-06e4-47a3-aac9-21cb806f3675" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="649a79cd-06e4-47a3-aac9-21cb806f3675">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3D6FD09-045A-4263-B935-31FAFD7A237D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="649a79cd-06e4-47a3-aac9-21cb806f3675"/>
+    <ds:schemaRef ds:uri="7f25b792-b2ba-4b5c-8669-b39a27555406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{663501A2-41E2-4171-A654-17AEE568C36A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F9D7643-B991-40B4-9569-D08A49A0FA61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f25b792-b2ba-4b5c-8669-b39a27555406"/>
+    <ds:schemaRef ds:uri="649a79cd-06e4-47a3-aac9-21cb806f3675"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>